<commit_message>
Dec 29 - gitignore updates
</commit_message>
<xml_diff>
--- a/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/Core.xlsx
+++ b/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/Core.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23607"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23621"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://guthyrenker.sharepoint.com/sites/ecommerce/Shared Documents/Merchandising Data Repo/CrepeErase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdesai\Guthy-Renker, LLC\ecommerce - Documents\Merchandising Data Repo\CrepeErase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="11_42D3077F6D93FD59E497D6A2753482042C73F92C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3346055D-B9D2-48F8-AD7C-4E7A8D36F774}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="11_42D3077F6D93FD59E497D6A2753482042C73F92C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8AC1D02A-E2E0-4A51-AD23-48CC3F6420D5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="20985" yWindow="-13230" windowWidth="7500" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Active Campaign" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="208">
   <si>
     <t>Vanity URL</t>
   </si>
@@ -483,7 +483,7 @@
     <t>Pre-Purchase Entry Promotion 6</t>
   </si>
   <si>
-    <t>Pre-Purchase Entry Renewal Plan</t>
+    <t>Pre-Purchase Entry Renewal Plan</t>
   </si>
   <si>
     <t>RCSA3V3</t>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>3-piece</t>
+  </si>
+  <si>
+    <t>Pre-Purchase Entry Renewal Plan</t>
   </si>
   <si>
     <t>One month after your first order is shipped, and then every three months thereafter, you will be sent a new full size supply of Crepe Erase®.Each shipment will be charged to the card you provide today, in three monthly payments at the low price of $54.95 plus $2.99 for shipping and handling per month,unless you call to cancel_x000D_
@@ -1866,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3487,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764EDFC1-17F3-43C1-9382-30B17CFE0B84}">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103:E103"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4762,17 +4765,17 @@
       <c r="A60" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="B60" s="55">
-        <v>59.95</v>
+      <c r="B60" s="57">
+        <v>11.97</v>
       </c>
       <c r="C60" s="57">
-        <v>39.950000000000003</v>
-      </c>
-      <c r="D60" s="55">
-        <v>59.95</v>
-      </c>
-      <c r="E60" s="58">
-        <v>39.950000000000003</v>
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="D60" s="57">
+        <v>11.97</v>
+      </c>
+      <c r="E60" s="57">
+        <v>8.9700000000000006</v>
       </c>
       <c r="F60" s="48"/>
       <c r="G60" s="35"/>
@@ -5219,7 +5222,7 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="61" t="s">
-        <v>148</v>
+        <v>202</v>
       </c>
       <c r="B81" s="62" t="s">
         <v>149</v>
@@ -5248,13 +5251,13 @@
         <v>154</v>
       </c>
       <c r="C82" s="66" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D82" s="66" t="s">
         <v>154</v>
       </c>
       <c r="E82" s="67" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F82" s="48"/>
       <c r="G82" s="35"/>
@@ -5501,13 +5504,13 @@
         <v>174</v>
       </c>
       <c r="C93" s="66" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D93" s="66" t="s">
         <v>174</v>
       </c>
       <c r="E93" s="67" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F93" s="48"/>
       <c r="G93" s="35"/>
@@ -5544,16 +5547,16 @@
         <v>179</v>
       </c>
       <c r="B95" s="66" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C95" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="D95" s="66" t="s">
         <v>206</v>
       </c>
-      <c r="D95" s="66" t="s">
-        <v>205</v>
-      </c>
       <c r="E95" s="66" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F95" s="48"/>
       <c r="G95" s="35"/>
@@ -5943,6 +5946,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5951,7 +5960,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C47EEB8100460B478BDC3BCCBE3D5051" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="829e995fc61fbfa25718206016b29da6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2" xmlns:ns3="3e63a3be-2d53-41f2-914e-dd0efc332534" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3545440ad2b936a9d10385f8b267d779" ns2:_="" ns3:_="">
     <xsd:import namespace="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2"/>
@@ -6116,20 +6125,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC58C8FE-5632-449B-B5BE-36F63AE51819}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D1CA06-B738-486D-9341-AA23A318022D}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E6203D-E6E6-4EA9-9DFF-6F77B7B5AC98}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC58C8FE-5632-449B-B5BE-36F63AE51819}"/>
 </file>
</xml_diff>

<commit_message>
Jan 5 - Updates
</commit_message>
<xml_diff>
--- a/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/Core.xlsx
+++ b/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/Core.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23621"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23702"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdesai\Guthy-Renker, LLC\ecommerce - Documents\Merchandising Data Repo\CrepeErase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="11_42D3077F6D93FD59E497D6A2753482042C73F92C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8AC1D02A-E2E0-4A51-AD23-48CC3F6420D5}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="11_42D3077F6D93FD59E497D6A2753482042C73F92C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{747B90B7-93C1-47D9-A6E0-70A0F2CBF74A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Active Campaign" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Version 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Active Campaign" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3490,7 +3490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764EDFC1-17F3-43C1-9382-30B17CFE0B84}">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
       <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>

</xml_diff>